<commit_message>
Update repos ex exit
@@
</commit_message>
<xml_diff>
--- a/reports/whooks-2023-09-20.xlsx
+++ b/reports/whooks-2023-09-20.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -481,7 +481,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>df4c70c4-fe09-4db6-a806-4cc01fce421e</v>
+        <v>57ceab23-bdbe-49e7-9718-a9a8fc14d23c</v>
       </c>
       <c r="B3" t="str">
         <v>reject</v>
@@ -490,30 +490,30 @@
         <v/>
       </c>
       <c r="D3" t="str">
-        <v>07c03600-5896-11ee-0040-f17e2c986ab3</v>
+        <v>d4ff5920-58a0-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E3" t="str">
-        <v>eric.sanchez@suvalsa.com</v>
+        <v>amolinar@unamsa.mx</v>
       </c>
       <c r="F3">
-        <v>1695311189</v>
+        <v>1695315828</v>
       </c>
       <c r="G3" t="str">
-        <v>07c11786-5896-11ee-81bf-0a58a9feac02</v>
+        <v>d50033ca-58a0-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H3" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I3" s="1">
-        <v>45190.40703976852</v>
+        <v>45190.46086008102</v>
       </c>
       <c r="J3" s="1">
-        <v>45190.40703976852</v>
+        <v>45190.46086008102</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>8a705ac5-72eb-432a-b342-eb28c47ecf3c</v>
+        <v>72bb16c8-35f4-43fe-9db7-a74f62396c36</v>
       </c>
       <c r="B4" t="str">
         <v>reject</v>
@@ -522,30 +522,30 @@
         <v/>
       </c>
       <c r="D4" t="str">
-        <v>372989d0-5893-11ee-0000-f1c69420d20b</v>
+        <v>61d79600-57c0-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E4" t="str">
-        <v>marisol.tlecuitl@grupocovico.mx</v>
+        <v>tramites@starseeds.com</v>
       </c>
       <c r="F4">
-        <v>1695309980</v>
+        <v>1695321828</v>
       </c>
       <c r="G4" t="str">
-        <v>372a1fda-5893-11ee-8862-0a58a9feac02</v>
+        <v>cd3c6426-58ae-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H4" t="str">
-        <v>hard bounce</v>
+        <v>hourly_rate_exceeded</v>
       </c>
       <c r="I4" s="1">
-        <v>45190.3931534838</v>
+        <v>45190.530301527775</v>
       </c>
       <c r="J4" s="1">
-        <v>45190.3931534838</v>
+        <v>45190.530301527775</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>f8b6c8bd-08b3-4547-b0d0-5e0e20372008</v>
+        <v>a996eddd-9062-4f7f-8cac-3a08a2ab2e7e</v>
       </c>
       <c r="B5" t="str">
         <v>reject</v>
@@ -554,30 +554,30 @@
         <v/>
       </c>
       <c r="D5" t="str">
-        <v>6d982b70-5893-11ee-0040-f17e2c986ab3</v>
+        <v>89265210-57d3-11ee-0000-f1c69420d20b</v>
       </c>
       <c r="E5" t="str">
-        <v>juan.gallegos@vinte.com</v>
+        <v>josezarate_af@outlook.com</v>
       </c>
       <c r="F5">
-        <v>1695310071</v>
+        <v>1695330014</v>
       </c>
       <c r="G5" t="str">
-        <v>6d98ff6d-5893-11ee-81bf-0a58a9feac02</v>
+        <v>dc8a53ea-58c1-11ee-8862-0a58a9feac02</v>
       </c>
       <c r="H5" t="str">
-        <v>hard bounce</v>
+        <v>hourly_rate_exceeded</v>
       </c>
       <c r="I5" s="1">
-        <v>45190.39419111111</v>
+        <v>45190.6250971875</v>
       </c>
       <c r="J5" s="1">
-        <v>45190.39419111111</v>
+        <v>45190.6250971875</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>771d6340-bf58-4639-ba1c-681201084dee</v>
+        <v>964365d1-a97b-4fb8-b377-65e09491d71c</v>
       </c>
       <c r="B6" t="str">
         <v>reject</v>
@@ -586,30 +586,30 @@
         <v/>
       </c>
       <c r="D6" t="str">
-        <v>6d95ba70-5893-11ee-0040-f17e2c986ab3</v>
+        <v>7568b230-57ca-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E6" t="str">
-        <v>isaac.mosco@vinte.com</v>
+        <v>jaimereyes@pumpingteam.com</v>
       </c>
       <c r="F6">
-        <v>1695310071</v>
+        <v>1695326116</v>
       </c>
       <c r="G6" t="str">
-        <v>6d971f94-5893-11ee-81bf-0a58a9feac02</v>
+        <v>c8dab542-58b8-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H6" t="str">
-        <v>hard bounce</v>
+        <v>hourly_rate_exceeded</v>
       </c>
       <c r="I6" s="1">
-        <v>45190.39419528935</v>
+        <v>45190.5799555787</v>
       </c>
       <c r="J6" s="1">
-        <v>45190.39419528935</v>
+        <v>45190.5799555787</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>9ebe13c4-de21-47b0-b797-f5fe1ad09dcf</v>
+        <v>df4c70c4-fe09-4db6-a806-4cc01fce421e</v>
       </c>
       <c r="B7" t="str">
         <v>reject</v>
@@ -618,30 +618,30 @@
         <v/>
       </c>
       <c r="D7" t="str">
-        <v>6d99d920-5893-11ee-0040-f17e2c986ab3</v>
+        <v>07c03600-5896-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E7" t="str">
-        <v>raul.delacruz@vinte.com</v>
+        <v>eric.sanchez@suvalsa.com</v>
       </c>
       <c r="F7">
-        <v>1695310071</v>
+        <v>1695311189</v>
       </c>
       <c r="G7" t="str">
-        <v>6d9ce308-5893-11ee-81bf-0a58a9feac02</v>
+        <v>07c11786-5896-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H7" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I7" s="1">
-        <v>45190.394195347224</v>
+        <v>45190.40703976852</v>
       </c>
       <c r="J7" s="1">
-        <v>45190.394195347224</v>
+        <v>45190.40703976852</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>669d4167-51db-49f0-a737-516be44f7dd1</v>
+        <v>db70e9aa-814e-476f-abcb-dfcf3682f02e</v>
       </c>
       <c r="B8" t="str">
         <v>reject</v>
@@ -650,30 +650,30 @@
         <v/>
       </c>
       <c r="D8" t="str">
-        <v>35e275c0-5891-11ee-0040-f17e2c986ab3</v>
+        <v>4c723560-57be-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E8" t="str">
-        <v>hortalizaspalmaso@hotmail.com</v>
+        <v>centralmonitoreo@grupoalimsa.com.mx</v>
       </c>
       <c r="F8">
-        <v>1695309119</v>
+        <v>1695320931</v>
       </c>
       <c r="G8" t="str">
-        <v>35e38c10-5891-11ee-81bf-0a58a9feac02</v>
+        <v>b69e4504-58ac-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H8" t="str">
-        <v>spam complaint</v>
+        <v>hourly_rate_exceeded</v>
       </c>
       <c r="I8" s="1">
-        <v>45190.38307979167</v>
+        <v>45190.51988528935</v>
       </c>
       <c r="J8" s="1">
-        <v>45190.38307979167</v>
+        <v>45190.51988528935</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>a23dcaa8-f3fc-4845-b7fb-4b1e53b6c64b</v>
+        <v>8a705ac5-72eb-432a-b342-eb28c47ecf3c</v>
       </c>
       <c r="B9" t="str">
         <v>reject</v>
@@ -682,30 +682,30 @@
         <v/>
       </c>
       <c r="D9" t="str">
-        <v>57fe7460-5891-11ee-0000-f1c69420d20b</v>
+        <v>372989d0-5893-11ee-0000-f1c69420d20b</v>
       </c>
       <c r="E9" t="str">
-        <v>inglectricadelcobre@hotmail.com</v>
+        <v>marisol.tlecuitl@grupocovico.mx</v>
       </c>
       <c r="F9">
-        <v>1695309176</v>
+        <v>1695309980</v>
       </c>
       <c r="G9" t="str">
-        <v>57ff4084-5891-11ee-8862-0a58a9feac02</v>
+        <v>372a1fda-5893-11ee-8862-0a58a9feac02</v>
       </c>
       <c r="H9" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I9" s="1">
-        <v>45190.38377422454</v>
+        <v>45190.3931534838</v>
       </c>
       <c r="J9" s="1">
-        <v>45190.38377422454</v>
+        <v>45190.3931534838</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>21d3f3b1-4a25-4cc9-aec3-1508dd25ebe8</v>
+        <v>459a09bf-3864-434b-91b2-b26860c44b0f</v>
       </c>
       <c r="B10" t="str">
         <v>reject</v>
@@ -714,30 +714,30 @@
         <v/>
       </c>
       <c r="D10" t="str">
-        <v>610083f0-5891-11ee-0000-f1c69420d20b</v>
+        <v>4e57be40-57be-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E10" t="str">
-        <v>t.ruvi@hotmail.com</v>
+        <v>monitoreo@grupoticsa.com</v>
       </c>
       <c r="F10">
-        <v>1695309191</v>
+        <v>1695320934</v>
       </c>
       <c r="G10" t="str">
-        <v>610154a6-5891-11ee-8862-0a58a9feac02</v>
+        <v>b82082a1-58ac-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H10" t="str">
-        <v>hard bounce</v>
+        <v>hourly_rate_exceeded</v>
       </c>
       <c r="I10" s="1">
-        <v>45190.38377434028</v>
+        <v>45190.51988555556</v>
       </c>
       <c r="J10" s="1">
-        <v>45190.38377434028</v>
+        <v>45190.51988555556</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>163a9217-3b78-421c-8d5c-e7bb521d6840</v>
+        <v>f8b6c8bd-08b3-4547-b0d0-5e0e20372008</v>
       </c>
       <c r="B11" t="str">
         <v>reject</v>
@@ -746,30 +746,30 @@
         <v/>
       </c>
       <c r="D11" t="str">
-        <v>60b1f1f0-5895-11ee-0040-f17e2c986ab3</v>
+        <v>6d982b70-5893-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E11" t="str">
-        <v>trafico@tubosyconexiones.com.mx</v>
+        <v>juan.gallegos@vinte.com</v>
       </c>
       <c r="F11">
-        <v>1695310909</v>
+        <v>1695310071</v>
       </c>
       <c r="G11" t="str">
-        <v>60b2e30a-5895-11ee-81bf-0a58a9feac02</v>
+        <v>6d98ff6d-5893-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H11" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I11" s="1">
-        <v>45190.40391743056</v>
+        <v>45190.39419111111</v>
       </c>
       <c r="J11" s="1">
-        <v>45190.40391743056</v>
+        <v>45190.39419111111</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>ed81cc49-6a9a-46b7-9830-8978627c5cfe</v>
+        <v>f324da00-d3c1-405f-9553-75b0b0d18cee</v>
       </c>
       <c r="B12" t="str">
         <v>reject</v>
@@ -778,30 +778,30 @@
         <v/>
       </c>
       <c r="D12" t="str">
-        <v>a39f4e20-5892-11ee-0040-f17e2c986ab3</v>
+        <v>bc0816d0-58ac-11ee-0000-f1c69420d20b</v>
       </c>
       <c r="E12" t="str">
-        <v>leonardosantana01@gmail.com</v>
+        <v>rvhernandez@hotmail.com</v>
       </c>
       <c r="F12">
-        <v>1695309732</v>
+        <v>1695320940</v>
       </c>
       <c r="G12" t="str">
-        <v>a3a03b1e-5892-11ee-81bf-0a58a9feac02</v>
+        <v>bc08bd1c-58ac-11ee-8862-0a58a9feac02</v>
       </c>
       <c r="H12" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I12" s="1">
-        <v>45190.390027546295</v>
+        <v>45190.519885601854</v>
       </c>
       <c r="J12" s="1">
-        <v>45190.390027546295</v>
+        <v>45190.519885601854</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>eded724c-986b-4524-b82e-e66a1f2158ff</v>
+        <v>771d6340-bf58-4639-ba1c-681201084dee</v>
       </c>
       <c r="B13" t="str">
         <v>reject</v>
@@ -810,30 +810,30 @@
         <v/>
       </c>
       <c r="D13" t="str">
-        <v>217a0e90-5896-11ee-0040-f17e2c986ab3</v>
+        <v>6d95ba70-5893-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E13" t="str">
-        <v>ccostosedif@promotoradehogares.com</v>
+        <v>isaac.mosco@vinte.com</v>
       </c>
       <c r="F13">
-        <v>1695311232</v>
+        <v>1695310071</v>
       </c>
       <c r="G13" t="str">
-        <v>217af2f0-5896-11ee-81bf-0a58a9feac02</v>
+        <v>6d971f94-5893-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H13" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I13" s="1">
-        <v>45190.40738827546</v>
+        <v>45190.39419528935</v>
       </c>
       <c r="J13" s="1">
-        <v>45190.40738827546</v>
+        <v>45190.39419528935</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>c2b05456-01eb-4438-b336-4a6e14d73d78</v>
+        <v>9ebe13c4-de21-47b0-b797-f5fe1ad09dcf</v>
       </c>
       <c r="B14" t="str">
         <v>reject</v>
@@ -842,30 +842,30 @@
         <v/>
       </c>
       <c r="D14" t="str">
-        <v>21763e00-5896-11ee-0040-f17e2c986ab3</v>
+        <v>6d99d920-5893-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E14" t="str">
-        <v>irios@promotoradehogares.com</v>
+        <v>raul.delacruz@vinte.com</v>
       </c>
       <c r="F14">
-        <v>1695311232</v>
+        <v>1695310071</v>
       </c>
       <c r="G14" t="str">
-        <v>21792f19-5896-11ee-81bf-0a58a9feac02</v>
+        <v>6d9ce308-5893-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H14" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I14" s="1">
-        <v>45190.40738834491</v>
+        <v>45190.394195347224</v>
       </c>
       <c r="J14" s="1">
-        <v>45190.40738834491</v>
+        <v>45190.394195347224</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>3dd8ac79-5177-4153-a5a4-fc2d903030c1</v>
+        <v>20bd8da9-0e8e-4bad-8f7d-0c74aa4c5b35</v>
       </c>
       <c r="B15" t="str">
         <v>reject</v>
@@ -874,30 +874,30 @@
         <v/>
       </c>
       <c r="D15" t="str">
-        <v>21d37930-5896-11ee-0000-f1c69420d20b</v>
+        <v>785bbf20-58a9-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E15" t="str">
-        <v>a.perez@laalemanamx.com</v>
+        <v>francisco.espinoza@logisticalocalq.com</v>
       </c>
       <c r="F15">
-        <v>1695311233</v>
+        <v>1695319538</v>
       </c>
       <c r="G15" t="str">
-        <v>21d42c19-5896-11ee-8862-0a58a9feac02</v>
+        <v>785cbc9e-58a9-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H15" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I15" s="1">
-        <v>45190.407388391206</v>
+        <v>45190.50356590278</v>
       </c>
       <c r="J15" s="1">
-        <v>45190.407388391206</v>
+        <v>45190.50356590278</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>f126e62f-65c2-4333-9ef7-31259daacfe1</v>
+        <v>669d4167-51db-49f0-a737-516be44f7dd1</v>
       </c>
       <c r="B16" t="str">
         <v>reject</v>
@@ -906,30 +906,30 @@
         <v/>
       </c>
       <c r="D16" t="str">
-        <v>c0d82d90-588d-11ee-0040-f17e2c986ab3</v>
+        <v>35e275c0-5891-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E16" t="str">
-        <v>ammontal@telmex.com</v>
+        <v>hortalizaspalmaso@hotmail.com</v>
       </c>
       <c r="F16">
-        <v>1695307634</v>
+        <v>1695309119</v>
       </c>
       <c r="G16" t="str">
-        <v>c0d8f189-588d-11ee-81bf-0a58a9feac02</v>
+        <v>35e38c10-5891-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H16" t="str">
-        <v>hard bounce</v>
+        <v>spam complaint</v>
       </c>
       <c r="I16" s="1">
-        <v>45190.37995835648</v>
+        <v>45190.38307979167</v>
       </c>
       <c r="J16" s="1">
-        <v>45190.37995835648</v>
+        <v>45190.38307979167</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>8e4956b5-041f-4a22-862b-fc01851976cf</v>
+        <v>83539095-633b-4793-82c8-88778fc26f44</v>
       </c>
       <c r="B17" t="str">
         <v>reject</v>
@@ -938,30 +938,30 @@
         <v/>
       </c>
       <c r="D17" t="str">
-        <v>b37f91f0-5889-11ee-0000-f1c69420d20b</v>
+        <v>159b9740-57cb-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E17" t="str">
-        <v>sapaza_arturo@sapaza.gob.mx</v>
+        <v>sistemas@sapaza.gob.mx</v>
       </c>
       <c r="F17">
-        <v>1695305894</v>
+        <v>1695326384</v>
       </c>
       <c r="G17" t="str">
-        <v>b3805b61-5889-11ee-8862-0a58a9feac02</v>
+        <v>69059fc8-58b9-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H17" t="str">
-        <v>hard bounce</v>
+        <v>hourly_rate_exceeded</v>
       </c>
       <c r="I17" s="1">
-        <v>45190.38065067129</v>
+        <v>45190.58307976852</v>
       </c>
       <c r="J17" s="1">
-        <v>45190.38065067129</v>
+        <v>45190.58307976852</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>42d596d2-c334-4436-9c7a-74b7a77036be</v>
+        <v>a23dcaa8-f3fc-4845-b7fb-4b1e53b6c64b</v>
       </c>
       <c r="B18" t="str">
         <v>reject</v>
@@ -970,30 +970,30 @@
         <v/>
       </c>
       <c r="D18" t="str">
-        <v>14a8c730-5899-11ee-0040-f17e2c986ab3</v>
+        <v>57fe7460-5891-11ee-0000-f1c69420d20b</v>
       </c>
       <c r="E18" t="str">
-        <v>meloperaciones@outlook.com</v>
+        <v>inglectricadelcobre@hotmail.com</v>
       </c>
       <c r="F18">
-        <v>1695312499</v>
+        <v>1695309176</v>
       </c>
       <c r="G18" t="str">
-        <v>14a989a9-5899-11ee-81bf-0a58a9feac02</v>
+        <v>57ff4084-5891-11ee-8862-0a58a9feac02</v>
       </c>
       <c r="H18" t="str">
-        <v>spam complaint</v>
+        <v>hard bounce</v>
       </c>
       <c r="I18" s="1">
-        <v>45190.42231841435</v>
+        <v>45190.38377422454</v>
       </c>
       <c r="J18" s="1">
-        <v>45190.42231841435</v>
+        <v>45190.38377422454</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>ce144598-a840-4092-afbb-169bce283b05</v>
+        <v>21d3f3b1-4a25-4cc9-aec3-1508dd25ebe8</v>
       </c>
       <c r="B19" t="str">
         <v>reject</v>
@@ -1002,30 +1002,30 @@
         <v/>
       </c>
       <c r="D19" t="str">
-        <v>20cdfed0-5890-11ee-0000-f1c69420d20b</v>
+        <v>610083f0-5891-11ee-0000-f1c69420d20b</v>
       </c>
       <c r="E19" t="str">
-        <v>monitoreo@adlenor.com</v>
+        <v>t.ruvi@hotmail.com</v>
       </c>
       <c r="F19">
-        <v>1695308654</v>
+        <v>1695309191</v>
       </c>
       <c r="G19" t="str">
-        <v>20cec561-5890-11ee-8862-0a58a9feac02</v>
+        <v>610154a6-5891-11ee-8862-0a58a9feac02</v>
       </c>
       <c r="H19" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I19" s="1">
-        <v>45190.38134712963</v>
+        <v>45190.38377434028</v>
       </c>
       <c r="J19" s="1">
-        <v>45190.38134712963</v>
+        <v>45190.38377434028</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>7fdbdd07-cb63-475c-8bb3-9ba32168ca41</v>
+        <v>163a9217-3b78-421c-8d5c-e7bb521d6840</v>
       </c>
       <c r="B20" t="str">
         <v>reject</v>
@@ -1034,30 +1034,30 @@
         <v/>
       </c>
       <c r="D20" t="str">
-        <v>22c8ef00-5891-11ee-0040-f17e2c986ab3</v>
+        <v>60b1f1f0-5895-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E20" t="str">
-        <v>asimbron@pcrent.com.mx</v>
+        <v>trafico@tubosyconexiones.com.mx</v>
       </c>
       <c r="F20">
-        <v>1695309087</v>
+        <v>1695310909</v>
       </c>
       <c r="G20" t="str">
-        <v>22c9c089-5891-11ee-81bf-0a58a9feac02</v>
+        <v>60b2e30a-5895-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H20" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I20" s="1">
-        <v>45190.382736770836</v>
+        <v>45190.40391743056</v>
       </c>
       <c r="J20" s="1">
-        <v>45190.382736770836</v>
+        <v>45190.40391743056</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>056c3d24-e86a-4056-8da5-bbffda85352e</v>
+        <v>d5ba4438-e61f-436f-9b3a-af7b6deae4a2</v>
       </c>
       <c r="B21" t="str">
         <v>reject</v>
@@ -1066,30 +1066,30 @@
         <v/>
       </c>
       <c r="D21" t="str">
-        <v>1cfffb50-589a-11ee-0000-f1c69420d20b</v>
+        <v>dde5e910-58ae-11ee-0000-f1c69420d20b</v>
       </c>
       <c r="E21" t="str">
-        <v>ventaspromesa@hotmail.com</v>
+        <v>sistemas@calibracionesime.com.mx</v>
       </c>
       <c r="F21">
-        <v>1695312942</v>
+        <v>1695321856</v>
       </c>
       <c r="G21" t="str">
-        <v>1d00bbcb-589a-11ee-8862-0a58a9feac02</v>
+        <v>dde76716-58ae-11ee-8862-0a58a9feac02</v>
       </c>
       <c r="H21" t="str">
-        <v>spam complaint</v>
+        <v>hard bounce</v>
       </c>
       <c r="I21" s="1">
-        <v>45190.427176006946</v>
+        <v>45190.53065209491</v>
       </c>
       <c r="J21" s="1">
-        <v>45190.427176006946</v>
+        <v>45190.53065209491</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>26c5ab0a-4a2b-4c0b-9843-459d0e41b002</v>
+        <v>f88453b2-d9d2-49e5-89f5-3a04d6eb5a53</v>
       </c>
       <c r="B22" t="str">
         <v>reject</v>
@@ -1098,30 +1098,30 @@
         <v/>
       </c>
       <c r="D22" t="str">
-        <v>8b99aab0-5891-11ee-0040-f17e2c986ab3</v>
+        <v>dd36ca10-58be-11ee-0000-f1c69420d20b</v>
       </c>
       <c r="E22" t="str">
-        <v>gerencia@cactustraffic.com.mx</v>
+        <v>rh@evocolor.com.mx</v>
       </c>
       <c r="F22">
-        <v>1695309263</v>
+        <v>1695328727</v>
       </c>
       <c r="G22" t="str">
-        <v>8b9a957f-5891-11ee-81bf-0a58a9feac02</v>
+        <v>dd3762cb-58be-11ee-8862-0a58a9feac02</v>
       </c>
       <c r="H22" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I22" s="1">
-        <v>45190.384819212966</v>
+        <v>45190.61016428241</v>
       </c>
       <c r="J22" s="1">
-        <v>45190.384819212966</v>
+        <v>45190.61016428241</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>bf82697e-0786-4f01-9147-cf40ac147c77</v>
+        <v>ed81cc49-6a9a-46b7-9830-8978627c5cfe</v>
       </c>
       <c r="B23" t="str">
         <v>reject</v>
@@ -1130,30 +1130,30 @@
         <v/>
       </c>
       <c r="D23" t="str">
-        <v>3c1b36b0-5892-11ee-0000-f1c69420d20b</v>
+        <v>a39f4e20-5892-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E23" t="str">
-        <v>hugo.hernandez@alteacorp.com</v>
+        <v>leonardosantana01@gmail.com</v>
       </c>
       <c r="F23">
-        <v>1695309559</v>
+        <v>1695309732</v>
       </c>
       <c r="G23" t="str">
-        <v>3c1bddcb-5892-11ee-8862-0a58a9feac02</v>
+        <v>a3a03b1e-5892-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H23" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I23" s="1">
-        <v>45190.388288090275</v>
+        <v>45190.390027546295</v>
       </c>
       <c r="J23" s="1">
-        <v>45190.388288090275</v>
+        <v>45190.390027546295</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>010bcb06-f784-4220-a47b-184f745a645a</v>
+        <v>eeb4b641-91dd-4a83-b086-d52353ea717a</v>
       </c>
       <c r="B24" t="str">
         <v>reject</v>
@@ -1162,30 +1162,30 @@
         <v/>
       </c>
       <c r="D24" t="str">
-        <v>3c198900-5892-11ee-0000-f1c69420d20b</v>
+        <v>5ee34640-58b2-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E24" t="str">
-        <v>aleli@alteacorp.com</v>
+        <v>rosyfloresbice@gmaill.com</v>
       </c>
       <c r="F24">
-        <v>1695309559</v>
+        <v>1695323361</v>
       </c>
       <c r="G24" t="str">
-        <v>3c1a45a2-5892-11ee-8862-0a58a9feac02</v>
+        <v>5ee455b4-58b2-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H24" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I24" s="1">
-        <v>45190.38829144676</v>
+        <v>45190.54801300926</v>
       </c>
       <c r="J24" s="1">
-        <v>45190.38829144676</v>
+        <v>45190.54801300926</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>09197482-341e-4a50-ab73-78741a6c26c5</v>
+        <v>6c5fe476-bf63-4201-a919-e09c59e1161e</v>
       </c>
       <c r="B25" t="str">
         <v>reject</v>
@@ -1194,30 +1194,30 @@
         <v/>
       </c>
       <c r="D25" t="str">
-        <v>47457d70-5892-11ee-0000-f1c69420d20b</v>
+        <v>ffaac080-57bd-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E25" t="str">
-        <v>creditoycobranza@liamco.com.mx</v>
+        <v>administracion@xtinfire.com</v>
       </c>
       <c r="F25">
-        <v>1695309577</v>
+        <v>1695320844</v>
       </c>
       <c r="G25" t="str">
-        <v>47463fb7-5892-11ee-8862-0a58a9feac02</v>
+        <v>82f57ecb-58ac-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H25" t="str">
-        <v>hard bounce</v>
+        <v>hourly_rate_exceeded</v>
       </c>
       <c r="I25" s="1">
-        <v>45190.38829149306</v>
+        <v>45190.518844872684</v>
       </c>
       <c r="J25" s="1">
-        <v>45190.38829149306</v>
+        <v>45190.518844872684</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>8ad2af84-546e-4fb4-8cad-324595a2eab3</v>
+        <v>eded724c-986b-4524-b82e-e66a1f2158ff</v>
       </c>
       <c r="B26" t="str">
         <v>reject</v>
@@ -1226,30 +1226,30 @@
         <v/>
       </c>
       <c r="D26" t="str">
-        <v>4748b1c0-5892-11ee-0040-f17e2c986ab3</v>
+        <v>217a0e90-5896-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E26" t="str">
-        <v>gerencia.operaciones@grupoliaco.com.mx</v>
+        <v>ccostosedif@promotoradehogares.com</v>
       </c>
       <c r="F26">
-        <v>1695309577</v>
+        <v>1695311232</v>
       </c>
       <c r="G26" t="str">
-        <v>474da78b-5892-11ee-81bf-0a58a9feac02</v>
+        <v>217af2f0-5896-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H26" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I26" s="1">
-        <v>45190.388291539355</v>
+        <v>45190.40738827546</v>
       </c>
       <c r="J26" s="1">
-        <v>45190.388291539355</v>
+        <v>45190.40738827546</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>2b2cb9ad-580b-4615-8833-a5daa27d6776</v>
+        <v>c2b05456-01eb-4438-b336-4a6e14d73d78</v>
       </c>
       <c r="B27" t="str">
         <v>reject</v>
@@ -1258,62 +1258,2846 @@
         <v/>
       </c>
       <c r="D27" t="str">
-        <v>4c051670-5894-11ee-0040-f17e2c986ab3</v>
+        <v>21763e00-5896-11ee-0040-f17e2c986ab3</v>
       </c>
       <c r="E27" t="str">
-        <v>alertas.backu@circulocorp.com</v>
+        <v>irios@promotoradehogares.com</v>
       </c>
       <c r="F27">
-        <v>1695310444</v>
+        <v>1695311232</v>
       </c>
       <c r="G27" t="str">
-        <v>4c05c6a3-5894-11ee-81bf-0a58a9feac02</v>
+        <v>21792f19-5896-11ee-81bf-0a58a9feac02</v>
       </c>
       <c r="H27" t="str">
         <v>hard bounce</v>
       </c>
       <c r="I27" s="1">
-        <v>45190.398357569444</v>
+        <v>45190.40738834491</v>
       </c>
       <c r="J27" s="1">
-        <v>45190.398357569444</v>
+        <v>45190.40738834491</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
+        <v>3dd8ac79-5177-4153-a5a4-fc2d903030c1</v>
+      </c>
+      <c r="B28" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C28" t="str">
+        <v/>
+      </c>
+      <c r="D28" t="str">
+        <v>21d37930-5896-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E28" t="str">
+        <v>a.perez@laalemanamx.com</v>
+      </c>
+      <c r="F28">
+        <v>1695311233</v>
+      </c>
+      <c r="G28" t="str">
+        <v>21d42c19-5896-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H28" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I28" s="1">
+        <v>45190.407388391206</v>
+      </c>
+      <c r="J28" s="1">
+        <v>45190.407388391206</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>f126e62f-65c2-4333-9ef7-31259daacfe1</v>
+      </c>
+      <c r="B29" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C29" t="str">
+        <v/>
+      </c>
+      <c r="D29" t="str">
+        <v>c0d82d90-588d-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E29" t="str">
+        <v>ammontal@telmex.com</v>
+      </c>
+      <c r="F29">
+        <v>1695307634</v>
+      </c>
+      <c r="G29" t="str">
+        <v>c0d8f189-588d-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H29" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I29" s="1">
+        <v>45190.37995835648</v>
+      </c>
+      <c r="J29" s="1">
+        <v>45190.37995835648</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>e7f98fec-4891-4748-9a83-7c4ac60f2a81</v>
+      </c>
+      <c r="B30" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C30" t="str">
+        <v/>
+      </c>
+      <c r="D30" t="str">
+        <v>0012f830-57be-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E30" t="str">
+        <v>subdireccion@xtinfire.com</v>
+      </c>
+      <c r="F30">
+        <v>1695320845</v>
+      </c>
+      <c r="G30" t="str">
+        <v>8349bf82-58ac-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H30" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I30" s="1">
+        <v>45190.518846990744</v>
+      </c>
+      <c r="J30" s="1">
+        <v>45190.518846990744</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>8e4956b5-041f-4a22-862b-fc01851976cf</v>
+      </c>
+      <c r="B31" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C31" t="str">
+        <v/>
+      </c>
+      <c r="D31" t="str">
+        <v>b37f91f0-5889-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E31" t="str">
+        <v>sapaza_arturo@sapaza.gob.mx</v>
+      </c>
+      <c r="F31">
+        <v>1695305894</v>
+      </c>
+      <c r="G31" t="str">
+        <v>b3805b61-5889-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H31" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I31" s="1">
+        <v>45190.38065067129</v>
+      </c>
+      <c r="J31" s="1">
+        <v>45190.38065067129</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>9f26f55e-9e99-4fce-acb5-57837648a9ec</v>
+      </c>
+      <c r="B32" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C32" t="str">
+        <v/>
+      </c>
+      <c r="D32" t="str">
+        <v>8690c930-57ca-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E32" t="str">
+        <v>juanbosco@sesco.mx</v>
+      </c>
+      <c r="F32">
+        <v>1695326144</v>
+      </c>
+      <c r="G32" t="str">
+        <v>d9fb3eb8-58b8-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H32" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I32" s="1">
+        <v>45190.58030560185</v>
+      </c>
+      <c r="J32" s="1">
+        <v>45190.58030560185</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>cf68767a-eeb9-4f2b-b371-34916518935d</v>
+      </c>
+      <c r="B33" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C33" t="str">
+        <v/>
+      </c>
+      <c r="D33" t="str">
+        <v>86933a30-57ca-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E33" t="str">
+        <v>control.vehicular@ferretodo.com.mx</v>
+      </c>
+      <c r="F33">
+        <v>1695326144</v>
+      </c>
+      <c r="G33" t="str">
+        <v>d9fdd697-58b8-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H33" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I33" s="1">
+        <v>45190.58030569444</v>
+      </c>
+      <c r="J33" s="1">
+        <v>45190.58030569444</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>42d596d2-c334-4436-9c7a-74b7a77036be</v>
+      </c>
+      <c r="B34" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C34" t="str">
+        <v/>
+      </c>
+      <c r="D34" t="str">
+        <v>14a8c730-5899-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E34" t="str">
+        <v>meloperaciones@outlook.com</v>
+      </c>
+      <c r="F34">
+        <v>1695312499</v>
+      </c>
+      <c r="G34" t="str">
+        <v>14a989a9-5899-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H34" t="str">
+        <v>spam complaint</v>
+      </c>
+      <c r="I34" s="1">
+        <v>45190.42231841435</v>
+      </c>
+      <c r="J34" s="1">
+        <v>45190.42231841435</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>ce144598-a840-4092-afbb-169bce283b05</v>
+      </c>
+      <c r="B35" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C35" t="str">
+        <v/>
+      </c>
+      <c r="D35" t="str">
+        <v>20cdfed0-5890-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E35" t="str">
+        <v>monitoreo@adlenor.com</v>
+      </c>
+      <c r="F35">
+        <v>1695308654</v>
+      </c>
+      <c r="G35" t="str">
+        <v>20cec561-5890-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H35" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I35" s="1">
+        <v>45190.38134712963</v>
+      </c>
+      <c r="J35" s="1">
+        <v>45190.38134712963</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>a7e8c253-9b84-489d-900c-3c3764b50044</v>
+      </c>
+      <c r="B36" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C36" t="str">
+        <v/>
+      </c>
+      <c r="D36" t="str">
+        <v>869f6f30-57ca-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E36" t="str">
+        <v>sjr@cactustraffic.com.mx</v>
+      </c>
+      <c r="F36">
+        <v>1695326144</v>
+      </c>
+      <c r="G36" t="str">
+        <v>da00de77-58b8-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H36" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I36" s="1">
+        <v>45190.58030574074</v>
+      </c>
+      <c r="J36" s="1">
+        <v>45190.58030574074</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>d6895347-748b-4e63-9c43-be5e19e04503</v>
+      </c>
+      <c r="B37" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C37" t="str">
+        <v/>
+      </c>
+      <c r="D37" t="str">
+        <v>57fcfb60-57ad-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E37" t="str">
+        <v>lbollain@proteinasmex.com.mx</v>
+      </c>
+      <c r="F37">
+        <v>1695313751</v>
+      </c>
+      <c r="G37" t="str">
+        <v>ff0a1629-589b-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H37" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I37" s="1">
+        <v>45190.43655054398</v>
+      </c>
+      <c r="J37" s="1">
+        <v>45190.43655054398</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>137683cc-b32e-4d05-b492-663041f244cb</v>
+      </c>
+      <c r="B38" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C38" t="str">
+        <v/>
+      </c>
+      <c r="D38" t="str">
+        <v>58103540-57ad-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E38" t="str">
+        <v>dalvarez@proteinasmex.com.mx</v>
+      </c>
+      <c r="F38">
+        <v>1695313751</v>
+      </c>
+      <c r="G38" t="str">
+        <v>ff0bb432-589b-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H38" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I38" s="1">
+        <v>45190.43655076389</v>
+      </c>
+      <c r="J38" s="1">
+        <v>45190.43655076389</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>314539e7-5de3-4884-9889-37e904911efc</v>
+      </c>
+      <c r="B39" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C39" t="str">
+        <v/>
+      </c>
+      <c r="D39" t="str">
+        <v>5808bb30-57ad-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E39" t="str">
+        <v>onavarrete@proteinasmex.com.mx</v>
+      </c>
+      <c r="F39">
+        <v>1695313751</v>
+      </c>
+      <c r="G39" t="str">
+        <v>ff0d24ec-589b-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H39" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I39" s="1">
+        <v>45190.43655079861</v>
+      </c>
+      <c r="J39" s="1">
+        <v>45190.43655079861</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>7fdbdd07-cb63-475c-8bb3-9ba32168ca41</v>
+      </c>
+      <c r="B40" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C40" t="str">
+        <v/>
+      </c>
+      <c r="D40" t="str">
+        <v>22c8ef00-5891-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E40" t="str">
+        <v>asimbron@pcrent.com.mx</v>
+      </c>
+      <c r="F40">
+        <v>1695309087</v>
+      </c>
+      <c r="G40" t="str">
+        <v>22c9c089-5891-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H40" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I40" s="1">
+        <v>45190.382736770836</v>
+      </c>
+      <c r="J40" s="1">
+        <v>45190.382736770836</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>ab037490-f050-4701-9bcb-524a42ed7614</v>
+      </c>
+      <c r="B41" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C41" t="str">
+        <v/>
+      </c>
+      <c r="D41" t="str">
+        <v>57f5cf70-57ad-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E41" t="str">
+        <v>acerezo@proteinasmex.com.mx</v>
+      </c>
+      <c r="F41">
+        <v>1695313751</v>
+      </c>
+      <c r="G41" t="str">
+        <v>ff0e1a92-589b-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H41" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I41" s="1">
+        <v>45190.43655385417</v>
+      </c>
+      <c r="J41" s="1">
+        <v>45190.43655385417</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>00950f42-bc05-426a-a832-71e14db0f64e</v>
+      </c>
+      <c r="B42" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C42" t="str">
+        <v/>
+      </c>
+      <c r="D42" t="str">
+        <v>57f88e90-57ad-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E42" t="str">
+        <v>vigilancia_oxalostoc@proteinasmex.com.mx</v>
+      </c>
+      <c r="F42">
+        <v>1695313751</v>
+      </c>
+      <c r="G42" t="str">
+        <v>ff12c202-589b-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H42" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I42" s="1">
+        <v>45190.436553900465</v>
+      </c>
+      <c r="J42" s="1">
+        <v>45190.436553900465</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>056c3d24-e86a-4056-8da5-bbffda85352e</v>
+      </c>
+      <c r="B43" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C43" t="str">
+        <v/>
+      </c>
+      <c r="D43" t="str">
+        <v>1cfffb50-589a-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E43" t="str">
+        <v>ventaspromesa@hotmail.com</v>
+      </c>
+      <c r="F43">
+        <v>1695312942</v>
+      </c>
+      <c r="G43" t="str">
+        <v>1d00bbcb-589a-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H43" t="str">
+        <v>spam complaint</v>
+      </c>
+      <c r="I43" s="1">
+        <v>45190.427176006946</v>
+      </c>
+      <c r="J43" s="1">
+        <v>45190.427176006946</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>26c5ab0a-4a2b-4c0b-9843-459d0e41b002</v>
+      </c>
+      <c r="B44" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C44" t="str">
+        <v/>
+      </c>
+      <c r="D44" t="str">
+        <v>8b99aab0-5891-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E44" t="str">
+        <v>gerencia@cactustraffic.com.mx</v>
+      </c>
+      <c r="F44">
+        <v>1695309263</v>
+      </c>
+      <c r="G44" t="str">
+        <v>8b9a957f-5891-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H44" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I44" s="1">
+        <v>45190.384819212966</v>
+      </c>
+      <c r="J44" s="1">
+        <v>45190.384819212966</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>bf82697e-0786-4f01-9147-cf40ac147c77</v>
+      </c>
+      <c r="B45" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C45" t="str">
+        <v/>
+      </c>
+      <c r="D45" t="str">
+        <v>3c1b36b0-5892-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E45" t="str">
+        <v>hugo.hernandez@alteacorp.com</v>
+      </c>
+      <c r="F45">
+        <v>1695309559</v>
+      </c>
+      <c r="G45" t="str">
+        <v>3c1bddcb-5892-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H45" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I45" s="1">
+        <v>45190.388288090275</v>
+      </c>
+      <c r="J45" s="1">
+        <v>45190.388288090275</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>010bcb06-f784-4220-a47b-184f745a645a</v>
+      </c>
+      <c r="B46" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C46" t="str">
+        <v/>
+      </c>
+      <c r="D46" t="str">
+        <v>3c198900-5892-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E46" t="str">
+        <v>aleli@alteacorp.com</v>
+      </c>
+      <c r="F46">
+        <v>1695309559</v>
+      </c>
+      <c r="G46" t="str">
+        <v>3c1a45a2-5892-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H46" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I46" s="1">
+        <v>45190.38829144676</v>
+      </c>
+      <c r="J46" s="1">
+        <v>45190.38829144676</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>09197482-341e-4a50-ab73-78741a6c26c5</v>
+      </c>
+      <c r="B47" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C47" t="str">
+        <v/>
+      </c>
+      <c r="D47" t="str">
+        <v>47457d70-5892-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E47" t="str">
+        <v>creditoycobranza@liamco.com.mx</v>
+      </c>
+      <c r="F47">
+        <v>1695309577</v>
+      </c>
+      <c r="G47" t="str">
+        <v>47463fb7-5892-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H47" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I47" s="1">
+        <v>45190.38829149306</v>
+      </c>
+      <c r="J47" s="1">
+        <v>45190.38829149306</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>8ad2af84-546e-4fb4-8cad-324595a2eab3</v>
+      </c>
+      <c r="B48" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C48" t="str">
+        <v/>
+      </c>
+      <c r="D48" t="str">
+        <v>4748b1c0-5892-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E48" t="str">
+        <v>gerencia.operaciones@grupoliaco.com.mx</v>
+      </c>
+      <c r="F48">
+        <v>1695309577</v>
+      </c>
+      <c r="G48" t="str">
+        <v>474da78b-5892-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H48" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I48" s="1">
+        <v>45190.388291539355</v>
+      </c>
+      <c r="J48" s="1">
+        <v>45190.388291539355</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>0b4c68f9-b79e-41b7-b0f5-c1b4cf725df0</v>
+      </c>
+      <c r="B49" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C49" t="str">
+        <v/>
+      </c>
+      <c r="D49" t="str">
+        <v>2fd68170-58a1-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E49" t="str">
+        <v>atencionaclientes@circulocorp.com</v>
+      </c>
+      <c r="F49">
+        <v>1695315981</v>
+      </c>
+      <c r="G49" t="str">
+        <v>2fd7350b-58a1-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H49" t="str">
+        <v>spam complaint</v>
+      </c>
+      <c r="I49" s="1">
+        <v>45190.46259695602</v>
+      </c>
+      <c r="J49" s="1">
+        <v>45190.46259695602</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>b4768c1e-fe96-4dbe-aee0-ce8464d99ae4</v>
+      </c>
+      <c r="B50" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C50" t="str">
+        <v/>
+      </c>
+      <c r="D50" t="str">
+        <v>34570080-58a1-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E50" t="str">
+        <v>jimenez_jesus.34@hotmail.com</v>
+      </c>
+      <c r="F50">
+        <v>1695315988</v>
+      </c>
+      <c r="G50" t="str">
+        <v>3457ae3e-58a1-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H50" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I50" s="1">
+        <v>45190.46259703704</v>
+      </c>
+      <c r="J50" s="1">
+        <v>45190.46259703704</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>0d56f9d7-2c18-4da3-90d8-0b2d0a767439</v>
+      </c>
+      <c r="B51" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C51" t="str">
+        <v/>
+      </c>
+      <c r="D51" t="str">
+        <v>15220c80-58b2-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E51" t="str">
+        <v>antonino.mor@hotmail.com</v>
+      </c>
+      <c r="F51">
+        <v>1695323237</v>
+      </c>
+      <c r="G51" t="str">
+        <v>1522da7c-58b2-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H51" t="str">
+        <v>spam complaint</v>
+      </c>
+      <c r="I51" s="1">
+        <v>45190.54662408565</v>
+      </c>
+      <c r="J51" s="1">
+        <v>45190.54662408565</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>e6cc6a8a-ce98-4695-a020-1d2bf2c52d51</v>
+      </c>
+      <c r="B52" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C52" t="str">
+        <v/>
+      </c>
+      <c r="D52" t="str">
+        <v>72ca65f0-58a1-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E52" t="str">
+        <v>mario.zarinana@jmg.com</v>
+      </c>
+      <c r="F52">
+        <v>1695316093</v>
+      </c>
+      <c r="G52" t="str">
+        <v>72cb64ec-58a1-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H52" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I52" s="1">
+        <v>45190.46363866898</v>
+      </c>
+      <c r="J52" s="1">
+        <v>45190.46363866898</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>117e20ac-a00f-46b4-b3db-e02042a9ca82</v>
+      </c>
+      <c r="B53" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C53" t="str">
+        <v/>
+      </c>
+      <c r="D53" t="str">
+        <v>9b436680-57ca-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E53" t="str">
+        <v>mespejo@elgaucho.com.mx</v>
+      </c>
+      <c r="F53">
+        <v>1695326179</v>
+      </c>
+      <c r="G53" t="str">
+        <v>eeb12aa4-58b8-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H53" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I53" s="1">
+        <v>45190.58064962963</v>
+      </c>
+      <c r="J53" s="1">
+        <v>45190.58064962963</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>4c98b567-0b9f-4f3d-88c4-bac4d22c1520</v>
+      </c>
+      <c r="B54" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C54" t="str">
+        <v/>
+      </c>
+      <c r="D54" t="str">
+        <v>c5876fc0-57c7-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E54" t="str">
+        <v>asistentedir@ciepacifico.com</v>
+      </c>
+      <c r="F54">
+        <v>1695324966</v>
+      </c>
+      <c r="G54" t="str">
+        <v>1b7ac26a-58b6-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H54" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I54" s="1">
+        <v>45190.56641318287</v>
+      </c>
+      <c r="J54" s="1">
+        <v>45190.56641318287</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>95fa8020-cf65-46d1-abef-3b87ceacfa97</v>
+      </c>
+      <c r="B55" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C55" t="str">
+        <v/>
+      </c>
+      <c r="D55" t="str">
+        <v>4913c820-57be-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E55" t="str">
+        <v>jose.sosa@sysctelecom.com.mx</v>
+      </c>
+      <c r="F55">
+        <v>1695320987</v>
+      </c>
+      <c r="G55" t="str">
+        <v>d8263e2b-58ac-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H55" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I55" s="1">
+        <v>45190.52057990741</v>
+      </c>
+      <c r="J55" s="1">
+        <v>45190.52057990741</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>2b2cb9ad-580b-4615-8833-a5daa27d6776</v>
+      </c>
+      <c r="B56" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C56" t="str">
+        <v/>
+      </c>
+      <c r="D56" t="str">
+        <v>4c051670-5894-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E56" t="str">
+        <v>alertas.backu@circulocorp.com</v>
+      </c>
+      <c r="F56">
+        <v>1695310444</v>
+      </c>
+      <c r="G56" t="str">
+        <v>4c05c6a3-5894-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H56" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I56" s="1">
+        <v>45190.398357569444</v>
+      </c>
+      <c r="J56" s="1">
+        <v>45190.398357569444</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>05260546-17e2-4b3f-80b8-8eb2f6743666</v>
+      </c>
+      <c r="B57" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C57" t="str">
+        <v/>
+      </c>
+      <c r="D57" t="str">
+        <v>49bf9880-57be-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E57" t="str">
+        <v>cmarrufo@juridicovales.com</v>
+      </c>
+      <c r="F57">
+        <v>1695320992</v>
+      </c>
+      <c r="G57" t="str">
+        <v>db002436-58ac-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H57" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I57" s="1">
+        <v>45190.52058016204</v>
+      </c>
+      <c r="J57" s="1">
+        <v>45190.52058016204</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>f6b717d9-defe-4c4c-832b-606ea5217980</v>
+      </c>
+      <c r="B58" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C58" t="str">
+        <v/>
+      </c>
+      <c r="D58" t="str">
+        <v>cb549760-58a9-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E58" t="str">
+        <v>contacto@iutsa.mx</v>
+      </c>
+      <c r="F58">
+        <v>1695319677</v>
+      </c>
+      <c r="G58" t="str">
+        <v>cb555c6a-58a9-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H58" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I58" s="1">
+        <v>45190.50530258102</v>
+      </c>
+      <c r="J58" s="1">
+        <v>45190.50530258102</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>67f2a171-4785-480a-92be-a89e92c3ae0a</v>
+      </c>
+      <c r="B59" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C59" t="str">
+        <v/>
+      </c>
+      <c r="D59" t="str">
+        <v>cb8d0a80-58bf-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E59" t="str">
+        <v>meixiueiro64@hotmail.com</v>
+      </c>
+      <c r="F59">
+        <v>1695329127</v>
+      </c>
+      <c r="G59" t="str">
+        <v>cb8dd4b5-58bf-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H59" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I59" s="1">
+        <v>45190.61467755787</v>
+      </c>
+      <c r="J59" s="1">
+        <v>45190.61467755787</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>087917f2-a335-41bc-a079-03e40801382c</v>
+      </c>
+      <c r="B60" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C60" t="str">
+        <v/>
+      </c>
+      <c r="D60" t="str">
+        <v>05892200-58a7-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E60" t="str">
+        <v>direccion@ayalaht.mx</v>
+      </c>
+      <c r="F60">
+        <v>1695318487</v>
+      </c>
+      <c r="G60" t="str">
+        <v>058a1846-58a7-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H60" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I60" s="1">
+        <v>45190.49141688657</v>
+      </c>
+      <c r="J60" s="1">
+        <v>45190.49141688657</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>42bfeebe-c306-4fac-931a-a7a9ea813773</v>
+      </c>
+      <c r="B61" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C61" t="str">
+        <v/>
+      </c>
+      <c r="D61" t="str">
+        <v>058acfb0-58a7-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E61" t="str">
+        <v>gerencia@ayalaht.mx</v>
+      </c>
+      <c r="F61">
+        <v>1695318487</v>
+      </c>
+      <c r="G61" t="str">
+        <v>058bb339-58a7-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H61" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I61" s="1">
+        <v>45190.49141695602</v>
+      </c>
+      <c r="J61" s="1">
+        <v>45190.49141695602</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>b4c3f413-6ae3-4482-b526-ec20ad184f8c</v>
+      </c>
+      <c r="B62" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C62" t="str">
+        <v/>
+      </c>
+      <c r="D62" t="str">
+        <v>dfaad830-57ca-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E62" t="str">
+        <v>supervision@homtex.com.mx</v>
+      </c>
+      <c r="F62">
+        <v>1695326294</v>
+      </c>
+      <c r="G62" t="str">
+        <v>33181319-58b9-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H62" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I62" s="1">
+        <v>45190.582042256945</v>
+      </c>
+      <c r="J62" s="1">
+        <v>45190.582042256945</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>3e6858ff-fee2-48ca-95e9-06536cfb6a9c</v>
+      </c>
+      <c r="B63" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C63" t="str">
+        <v/>
+      </c>
+      <c r="D63" t="str">
+        <v>12f2fb90-57c2-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E63" t="str">
+        <v>sistemas@tubosyconexiones.mx</v>
+      </c>
+      <c r="F63">
+        <v>1695322515</v>
+      </c>
+      <c r="G63" t="str">
+        <v>665fcea9-58b0-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H63" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I63" s="1">
+        <v>45190.53829178241</v>
+      </c>
+      <c r="J63" s="1">
+        <v>45190.53829178241</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>d3511cad-a9e4-49cf-8140-3cf9923b128c</v>
+      </c>
+      <c r="B64" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C64" t="str">
+        <v/>
+      </c>
+      <c r="D64" t="str">
+        <v>12f21130-57c2-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E64" t="str">
+        <v>auditoria@tubosyconexiones.mx</v>
+      </c>
+      <c r="F64">
+        <v>1695322515</v>
+      </c>
+      <c r="G64" t="str">
+        <v>66611f29-58b0-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H64" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I64" s="1">
+        <v>45190.538291840276</v>
+      </c>
+      <c r="J64" s="1">
+        <v>45190.538291840276</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>8919304e-b6e4-4460-88e0-53843686cb1f</v>
+      </c>
+      <c r="B65" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C65" t="str">
+        <v/>
+      </c>
+      <c r="D65" t="str">
+        <v>b3f78670-589c-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E65" t="str">
+        <v>tere.cruz@ccptelcel.com.mx</v>
+      </c>
+      <c r="F65">
+        <v>1695314055</v>
+      </c>
+      <c r="G65" t="str">
+        <v>b3f9c33a-589c-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H65" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I65" s="1">
+        <v>45190.44037447916</v>
+      </c>
+      <c r="J65" s="1">
+        <v>45190.44037447916</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>c19dd307-97b7-4e2b-8032-9c584163b16d</v>
+      </c>
+      <c r="B66" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C66" t="str">
+        <v/>
+      </c>
+      <c r="D66" t="str">
+        <v>1425fd50-57c2-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E66" t="str">
+        <v>transportesmontesdeoca@hotmail.com</v>
+      </c>
+      <c r="F66">
+        <v>1695322516</v>
+      </c>
+      <c r="G66" t="str">
+        <v>678bc27b-58b0-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H66" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I66" s="1">
+        <v>45190.538291875</v>
+      </c>
+      <c r="J66" s="1">
+        <v>45190.538291875</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>ccd01f25-37f0-4f02-8208-2f8fff5f2f8a</v>
+      </c>
+      <c r="B67" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C67" t="str">
+        <v/>
+      </c>
+      <c r="D67" t="str">
+        <v>14275ce0-57c2-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E67" t="str">
+        <v>aaronalejandrosantanacalderon@gmail.com</v>
+      </c>
+      <c r="F67">
+        <v>1695322517</v>
+      </c>
+      <c r="G67" t="str">
+        <v>678fb773-58b0-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H67" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I67" s="1">
+        <v>45190.53829192129</v>
+      </c>
+      <c r="J67" s="1">
+        <v>45190.53829192129</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
         <v>7345613e-4c0b-43f5-8cf2-785db4fa60d9</v>
       </c>
-      <c r="B28" t="str">
-        <v>reject</v>
-      </c>
-      <c r="C28" t="str">
-        <v/>
-      </c>
-      <c r="D28" t="str">
+      <c r="B68" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C68" t="str">
+        <v/>
+      </c>
+      <c r="D68" t="str">
         <v>45d9bed0-589a-11ee-0040-f17e2c986ab3</v>
       </c>
-      <c r="E28" t="str">
+      <c r="E68" t="str">
         <v>contolinterno@oppsiservicios.com.mx</v>
       </c>
-      <c r="F28">
+      <c r="F68">
         <v>1695313011</v>
       </c>
-      <c r="G28" t="str">
+      <c r="G68" t="str">
         <v>45daae22-589a-11ee-81bf-0a58a9feac02</v>
       </c>
-      <c r="H28" t="str">
-        <v>hard bounce</v>
-      </c>
-      <c r="I28" s="1">
+      <c r="H68" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I68" s="1">
         <v>45190.428220925925</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J68" s="1">
         <v>45190.428220925925</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>f94e18b2-3393-43d2-a049-a9a1ae5870c9</v>
+      </c>
+      <c r="B69" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C69" t="str">
+        <v/>
+      </c>
+      <c r="D69" t="str">
+        <v>3738b800-57c2-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E69" t="str">
+        <v>ju_cfm@outlook.com</v>
+      </c>
+      <c r="F69">
+        <v>1695322575</v>
+      </c>
+      <c r="G69" t="str">
+        <v>8aac1d51-58b0-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H69" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I69" s="1">
+        <v>45190.538986238425</v>
+      </c>
+      <c r="J69" s="1">
+        <v>45190.538986238425</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>57d4d29c-1c17-463c-acbc-f247d3903e2a</v>
+      </c>
+      <c r="B70" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C70" t="str">
+        <v/>
+      </c>
+      <c r="D70" t="str">
+        <v>5afa2940-57c2-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E70" t="str">
+        <v>flotilladelza@gmail.com</v>
+      </c>
+      <c r="F70">
+        <v>1695322635</v>
+      </c>
+      <c r="G70" t="str">
+        <v>ae6174a1-58b0-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H70" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I70" s="1">
+        <v>45190.53967646991</v>
+      </c>
+      <c r="J70" s="1">
+        <v>45190.53967646991</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>d1a77359-2a9d-4937-a616-da99a24573a1</v>
+      </c>
+      <c r="B71" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C71" t="str">
+        <v/>
+      </c>
+      <c r="D71" t="str">
+        <v>5afc7330-57c2-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E71" t="str">
+        <v>karen@grupodelza.com</v>
+      </c>
+      <c r="F71">
+        <v>1695322635</v>
+      </c>
+      <c r="G71" t="str">
+        <v>ae71cb32-58b0-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H71" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I71" s="1">
+        <v>45190.539676608794</v>
+      </c>
+      <c r="J71" s="1">
+        <v>45190.539676608794</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>421a433a-f544-4eb8-a567-b35666d7c652</v>
+      </c>
+      <c r="B72" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C72" t="str">
+        <v/>
+      </c>
+      <c r="D72" t="str">
+        <v>5afe9610-57c2-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E72" t="str">
+        <v>noe@grupodelza.com</v>
+      </c>
+      <c r="F72">
+        <v>1695322635</v>
+      </c>
+      <c r="G72" t="str">
+        <v>ae6ebb03-58b0-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H72" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I72" s="1">
+        <v>45190.53968002315</v>
+      </c>
+      <c r="J72" s="1">
+        <v>45190.53968002315</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>0ba157ce-34f3-4b0e-ad1e-27f6b8fc9da2</v>
+      </c>
+      <c r="B73" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C73" t="str">
+        <v/>
+      </c>
+      <c r="D73" t="str">
+        <v>5afd84a0-57c2-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E73" t="str">
+        <v>nquezada@grupodelza.com</v>
+      </c>
+      <c r="F73">
+        <v>1695322635</v>
+      </c>
+      <c r="G73" t="str">
+        <v>ae6da49d-58b0-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H73" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I73" s="1">
+        <v>45190.539680104164</v>
+      </c>
+      <c r="J73" s="1">
+        <v>45190.539680104164</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>bbc3a710-cb51-4312-bb9b-7e12d17735fc</v>
+      </c>
+      <c r="B74" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C74" t="str">
+        <v/>
+      </c>
+      <c r="D74" t="str">
+        <v>2a3ac2d0-58ab-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E74" t="str">
+        <v>resmeralda@elsoldesanluis.com.mx</v>
+      </c>
+      <c r="F74">
+        <v>1695320266</v>
+      </c>
+      <c r="G74" t="str">
+        <v>2a3b8180-58ab-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H74" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I74" s="1">
+        <v>45190.512246701386</v>
+      </c>
+      <c r="J74" s="1">
+        <v>45190.512246701386</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>b49465e9-4165-472b-9dc6-651991d0dfe2</v>
+      </c>
+      <c r="B75" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C75" t="str">
+        <v/>
+      </c>
+      <c r="D75" t="str">
+        <v>a14b9b50-58ac-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E75" t="str">
+        <v>canto@corrocionyproteccion.com</v>
+      </c>
+      <c r="F75">
+        <v>1695320895</v>
+      </c>
+      <c r="G75" t="str">
+        <v>a14c6e08-58ac-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H75" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I75" s="1">
+        <v>45190.519538217595</v>
+      </c>
+      <c r="J75" s="1">
+        <v>45190.519538217595</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>e610bfe2-2c45-4483-b88c-a1c281d1635a</v>
+      </c>
+      <c r="B76" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C76" t="str">
+        <v/>
+      </c>
+      <c r="D76" t="str">
+        <v>510db680-57be-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E76" t="str">
+        <v>vanzel@outook.es</v>
+      </c>
+      <c r="F76">
+        <v>1695320901</v>
+      </c>
+      <c r="G76" t="str">
+        <v>a489e034-58ac-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H76" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I76" s="1">
+        <v>45190.51953849537</v>
+      </c>
+      <c r="J76" s="1">
+        <v>45190.51953849537</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>5ffdbed7-ec44-4ebd-9787-ccebea51e269</v>
+      </c>
+      <c r="B77" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C77" t="str">
+        <v/>
+      </c>
+      <c r="D77" t="str">
+        <v>a14d9720-58ac-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E77" t="str">
+        <v>hrivera@corrocionyproteccion.com</v>
+      </c>
+      <c r="F77">
+        <v>1695320895</v>
+      </c>
+      <c r="G77" t="str">
+        <v>a14e4b54-58ac-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H77" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I77" s="1">
+        <v>45190.51954142361</v>
+      </c>
+      <c r="J77" s="1">
+        <v>45190.51954142361</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>0e45b1e4-c466-4b7c-93e7-f8afa0736002</v>
+      </c>
+      <c r="B78" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C78" t="str">
+        <v/>
+      </c>
+      <c r="D78" t="str">
+        <v>aae26c80-57ca-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E78" t="str">
+        <v>ing_ballesterosr@hotmail.com</v>
+      </c>
+      <c r="F78">
+        <v>1695326205</v>
+      </c>
+      <c r="G78" t="str">
+        <v>fe438d46-58b8-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H78" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I78" s="1">
+        <v>45190.58099973379</v>
+      </c>
+      <c r="J78" s="1">
+        <v>45190.58099973379</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>d0f036c3-3856-4a3e-b278-0e914d20ed6e</v>
+      </c>
+      <c r="B79" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C79" t="str">
+        <v/>
+      </c>
+      <c r="D79" t="str">
+        <v>f2c98f10-57ca-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E79" t="str">
+        <v>monitoreo@pylsa.com</v>
+      </c>
+      <c r="F79">
+        <v>1695326326</v>
+      </c>
+      <c r="G79" t="str">
+        <v>462ae813-58b9-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H79" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I79" s="1">
+        <v>45190.58238820602</v>
+      </c>
+      <c r="J79" s="1">
+        <v>45190.58238820602</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>ad4db05e-d9c8-436e-8696-b4ac970e8ef2</v>
+      </c>
+      <c r="B80" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C80" t="str">
+        <v/>
+      </c>
+      <c r="D80" t="str">
+        <v>df69d480-58af-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E80" t="str">
+        <v>admon@iluminaciondelnoreste.com</v>
+      </c>
+      <c r="F80">
+        <v>1695322288</v>
+      </c>
+      <c r="G80" t="str">
+        <v>df6aa1fe-58af-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H80" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I80" s="1">
+        <v>45190.535514097224</v>
+      </c>
+      <c r="J80" s="1">
+        <v>45190.535514097224</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>146594bd-3df0-4a37-b057-daf42816e586</v>
+      </c>
+      <c r="B81" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C81" t="str">
+        <v/>
+      </c>
+      <c r="D81" t="str">
+        <v>2b97a480-57cb-11ee-0041-f17e2c986ab3</v>
+      </c>
+      <c r="E81" t="str">
+        <v>gizaccaro@gmail.com</v>
+      </c>
+      <c r="F81">
+        <v>1695326421</v>
+      </c>
+      <c r="G81" t="str">
+        <v>7f01be98-58b9-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H81" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I81" s="1">
+        <v>45190.58342702546</v>
+      </c>
+      <c r="J81" s="1">
+        <v>45190.58342702546</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>afd8d9e8-4a90-4396-80c7-8a8a2c353b4f</v>
+      </c>
+      <c r="B82" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C82" t="str">
+        <v/>
+      </c>
+      <c r="D82" t="str">
+        <v>2b992b20-57cb-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E82" t="str">
+        <v>meli.ortega@asiarobotica.com</v>
+      </c>
+      <c r="F82">
+        <v>1695326421</v>
+      </c>
+      <c r="G82" t="str">
+        <v>7f0f35f7-58b9-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H82" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I82" s="1">
+        <v>45190.58342724537</v>
+      </c>
+      <c r="J82" s="1">
+        <v>45190.58342724537</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>89a591f1-2ee6-4d3d-b758-9edd0c31a8f7</v>
+      </c>
+      <c r="B83" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C83" t="str">
+        <v/>
+      </c>
+      <c r="D83" t="str">
+        <v>8b111d00-57d1-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E83" t="str">
+        <v>ventas@eilsa.mx</v>
+      </c>
+      <c r="F83">
+        <v>1695329162</v>
+      </c>
+      <c r="G83" t="str">
+        <v>e06807cd-58bf-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H83" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I83" s="1">
+        <v>45190.61502837963</v>
+      </c>
+      <c r="J83" s="1">
+        <v>45190.61502837963</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>fc34782c-9d4c-49d6-b3a7-706f4b4dbca9</v>
+      </c>
+      <c r="B84" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C84" t="str">
+        <v/>
+      </c>
+      <c r="D84" t="str">
+        <v>26bfa5b0-57c2-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E84" t="str">
+        <v>mruiz@parkercorp.com.mx</v>
+      </c>
+      <c r="F84">
+        <v>1695322548</v>
+      </c>
+      <c r="G84" t="str">
+        <v>7a29301d-58b0-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H84" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I84" s="1">
+        <v>45190.53863663194</v>
+      </c>
+      <c r="J84" s="1">
+        <v>45190.53863663194</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>8586d749-0f40-415f-bf2f-36545c71c1e0</v>
+      </c>
+      <c r="B85" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C85" t="str">
+        <v/>
+      </c>
+      <c r="D85" t="str">
+        <v>26c0b720-57c2-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E85" t="str">
+        <v>jpantoja@parkercorp.com.mx</v>
+      </c>
+      <c r="F85">
+        <v>1695322548</v>
+      </c>
+      <c r="G85" t="str">
+        <v>7a256ebf-58b0-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H85" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I85" s="1">
+        <v>45190.53863689815</v>
+      </c>
+      <c r="J85" s="1">
+        <v>45190.53863689815</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>a478db5a-61b7-4cea-820e-08d40dc36e57</v>
+      </c>
+      <c r="B86" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C86" t="str">
+        <v/>
+      </c>
+      <c r="D86" t="str">
+        <v>26bc2340-57c2-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E86" t="str">
+        <v>agalindo@parkercorp.com.mx</v>
+      </c>
+      <c r="F86">
+        <v>1695322548</v>
+      </c>
+      <c r="G86" t="str">
+        <v>7a2479f8-58b0-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H86" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I86" s="1">
+        <v>45190.53863693287</v>
+      </c>
+      <c r="J86" s="1">
+        <v>45190.53863693287</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>f6801f62-9049-4816-bc86-5b4ec8ec7343</v>
+      </c>
+      <c r="B87" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C87" t="str">
+        <v/>
+      </c>
+      <c r="D87" t="str">
+        <v>28146040-57c2-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E87" t="str">
+        <v>raulh.truckexpress@gmail.com</v>
+      </c>
+      <c r="F87">
+        <v>1695322550</v>
+      </c>
+      <c r="G87" t="str">
+        <v>7b756cf1-58b0-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H87" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I87" s="1">
+        <v>45190.53863696759</v>
+      </c>
+      <c r="J87" s="1">
+        <v>45190.53863696759</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>af316aea-defa-4943-bdf6-9e21ff752f54</v>
+      </c>
+      <c r="B88" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C88" t="str">
+        <v/>
+      </c>
+      <c r="D88" t="str">
+        <v>2a9ae410-57c2-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E88" t="str">
+        <v>monitoreo@geb.mx</v>
+      </c>
+      <c r="F88">
+        <v>1695322554</v>
+      </c>
+      <c r="G88" t="str">
+        <v>7dfc1126-58b0-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H88" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I88" s="1">
+        <v>45190.53863700231</v>
+      </c>
+      <c r="J88" s="1">
+        <v>45190.53863700231</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>ab7929eb-a714-4993-a1b5-b855c232f2ef</v>
+      </c>
+      <c r="B89" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C89" t="str">
+        <v/>
+      </c>
+      <c r="D89" t="str">
+        <v>498292b0-57c2-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E89" t="str">
+        <v>gpsmormex2019@gmail.com</v>
+      </c>
+      <c r="F89">
+        <v>1695322606</v>
+      </c>
+      <c r="G89" t="str">
+        <v>9ce40dac-58b0-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H89" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I89" s="1">
+        <v>45190.539333229164</v>
+      </c>
+      <c r="J89" s="1">
+        <v>45190.539333229164</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>26fbfb7c-d621-459a-a51b-dc58be9cb7bb</v>
+      </c>
+      <c r="B90" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C90" t="str">
+        <v/>
+      </c>
+      <c r="D90" t="str">
+        <v>6c3e53c0-57c2-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E90" t="str">
+        <v>galvanmary71@hotmail.com</v>
+      </c>
+      <c r="F90">
+        <v>1695322664</v>
+      </c>
+      <c r="G90" t="str">
+        <v>bfaa1f9d-58b0-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H90" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I90" s="1">
+        <v>45190.54002363426</v>
+      </c>
+      <c r="J90" s="1">
+        <v>45190.54002363426</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>757e31ee-f679-4462-9c36-026f7c790544</v>
+      </c>
+      <c r="B91" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C91" t="str">
+        <v/>
+      </c>
+      <c r="D91" t="str">
+        <v>6d1b1f30-57c2-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E91" t="str">
+        <v>erick.castillo@simasmyf.gob.mx</v>
+      </c>
+      <c r="F91">
+        <v>1695322666</v>
+      </c>
+      <c r="G91" t="str">
+        <v>c085ac0c-58b0-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H91" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I91" s="1">
+        <v>45190.54002375</v>
+      </c>
+      <c r="J91" s="1">
+        <v>45190.54002375</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>1366d8bc-ddbb-47d9-8f0a-4227b8889fa3</v>
+      </c>
+      <c r="B92" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C92" t="str">
+        <v/>
+      </c>
+      <c r="D92" t="str">
+        <v>6e323480-57c2-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E92" t="str">
+        <v>sistemas@paisallantas.com.mx</v>
+      </c>
+      <c r="F92">
+        <v>1695322668</v>
+      </c>
+      <c r="G92" t="str">
+        <v>c1a2a858-58b0-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H92" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I92" s="1">
+        <v>45190.540023773145</v>
+      </c>
+      <c r="J92" s="1">
+        <v>45190.540023773145</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>3c30f104-a07d-4c69-be42-35aac501cf9c</v>
+      </c>
+      <c r="B93" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C93" t="str">
+        <v/>
+      </c>
+      <c r="D93" t="str">
+        <v>6c3b6d90-57c2-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E93" t="str">
+        <v>gruiz.zpc@gmail.com</v>
+      </c>
+      <c r="F93">
+        <v>1695322664</v>
+      </c>
+      <c r="G93" t="str">
+        <v>bfa54ede-58b0-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H93" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I93" s="1">
+        <v>45190.54002695602</v>
+      </c>
+      <c r="J93" s="1">
+        <v>45190.54002695602</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>9f43751c-7311-4aa4-893a-1168515dd1b6</v>
+      </c>
+      <c r="B94" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C94" t="str">
+        <v/>
+      </c>
+      <c r="D94" t="str">
+        <v>7fd17750-57c2-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E94" t="str">
+        <v>armando.sarmiento@bierzo.com.mx</v>
+      </c>
+      <c r="F94">
+        <v>1695322697</v>
+      </c>
+      <c r="G94" t="str">
+        <v>d3364e18-58b0-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H94" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I94" s="1">
+        <v>45190.54037099537</v>
+      </c>
+      <c r="J94" s="1">
+        <v>45190.54037099537</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>f28c75da-ae83-40e8-b062-d56a389cc9af</v>
+      </c>
+      <c r="B95" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C95" t="str">
+        <v/>
+      </c>
+      <c r="D95" t="str">
+        <v>91c8c530-57c2-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E95" t="str">
+        <v>alarmagps@pylsa.com</v>
+      </c>
+      <c r="F95">
+        <v>1695322727</v>
+      </c>
+      <c r="G95" t="str">
+        <v>e532f275-58b0-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H95" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I95" s="1">
+        <v>45190.54072135417</v>
+      </c>
+      <c r="J95" s="1">
+        <v>45190.54072135417</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>9b15109f-b3ad-4f9f-b15a-4e4f2519fd66</v>
+      </c>
+      <c r="B96" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C96" t="str">
+        <v/>
+      </c>
+      <c r="D96" t="str">
+        <v>a18d5490-57c2-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E96" t="str">
+        <v>m.escobedoproteinas@gmail.com</v>
+      </c>
+      <c r="F96">
+        <v>1695322754</v>
+      </c>
+      <c r="G96" t="str">
+        <v>f4f19cd1-58b0-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H96" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I96" s="1">
+        <v>45190.54106552083</v>
+      </c>
+      <c r="J96" s="1">
+        <v>45190.54106552083</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>218b9f22-702d-4367-a4ad-93ae0826c843</v>
+      </c>
+      <c r="B97" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C97" t="str">
+        <v/>
+      </c>
+      <c r="D97" t="str">
+        <v>0d27a190-58b5-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E97" t="str">
+        <v>licluluclemente@trascoro.com</v>
+      </c>
+      <c r="F97">
+        <v>1695324512</v>
+      </c>
+      <c r="G97" t="str">
+        <v>0d284dad-58b5-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H97" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I97" s="1">
+        <v>45190.5612040162</v>
+      </c>
+      <c r="J97" s="1">
+        <v>45190.5612040162</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>0174eff1-11f9-4201-b31f-698cb55a7d06</v>
+      </c>
+      <c r="B98" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C98" t="str">
+        <v/>
+      </c>
+      <c r="D98" t="str">
+        <v>0d290120-58b5-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E98" t="str">
+        <v>rcontreras@trascoro.com</v>
+      </c>
+      <c r="F98">
+        <v>1695324512</v>
+      </c>
+      <c r="G98" t="str">
+        <v>0d29d733-58b5-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H98" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I98" s="1">
+        <v>45190.56120420139</v>
+      </c>
+      <c r="J98" s="1">
+        <v>45190.56120420139</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>0ca33cb9-a9f4-4005-8510-c6ff07181127</v>
+      </c>
+      <c r="B99" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C99" t="str">
+        <v/>
+      </c>
+      <c r="D99" t="str">
+        <v>b71fa380-57c2-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E99" t="str">
+        <v>flotillagf@gmail.com</v>
+      </c>
+      <c r="F99">
+        <v>1695322790</v>
+      </c>
+      <c r="G99" t="str">
+        <v>0a840c29-58b1-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H99" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I99" s="1">
+        <v>45190.54141579861</v>
+      </c>
+      <c r="J99" s="1">
+        <v>45190.54141579861</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>ac1353f4-6415-4b9a-9eb9-9c33686532fa</v>
+      </c>
+      <c r="B100" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C100" t="str">
+        <v/>
+      </c>
+      <c r="D100" t="str">
+        <v>72ee2a80-58b5-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E100" t="str">
+        <v>gsalddierna@trascoro.com</v>
+      </c>
+      <c r="F100">
+        <v>1695324683</v>
+      </c>
+      <c r="G100" t="str">
+        <v>72ef0713-58b5-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H100" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I100" s="1">
+        <v>45190.563290694445</v>
+      </c>
+      <c r="J100" s="1">
+        <v>45190.563290694445</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>cd96a396-428c-4562-b5c5-e3f87d69a25f</v>
+      </c>
+      <c r="B101" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C101" t="str">
+        <v/>
+      </c>
+      <c r="D101" t="str">
+        <v>bc34a0c0-57ca-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E101" t="str">
+        <v>contablegks@gmail.com</v>
+      </c>
+      <c r="F101">
+        <v>1695326234</v>
+      </c>
+      <c r="G101" t="str">
+        <v>0f96090f-58b9-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H101" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I101" s="1">
+        <v>45190.58134344908</v>
+      </c>
+      <c r="J101" s="1">
+        <v>45190.58134344908</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>2a9b198d-69aa-4ddd-96a5-7f88610a145c</v>
+      </c>
+      <c r="B102" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C102" t="str">
+        <v/>
+      </c>
+      <c r="D102" t="str">
+        <v>9e14bbd0-58c3-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E102" t="str">
+        <v>jjta48@hotmail.com</v>
+      </c>
+      <c r="F102">
+        <v>1695330768</v>
+      </c>
+      <c r="G102" t="str">
+        <v>9e15dd64-58c3-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H102" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I102" s="1">
+        <v>45190.63376619213</v>
+      </c>
+      <c r="J102" s="1">
+        <v>45190.63376619213</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>f368a77b-e7ab-4150-bfcd-0ca753f76daf</v>
+      </c>
+      <c r="B103" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C103" t="str">
+        <v/>
+      </c>
+      <c r="D103" t="str">
+        <v>a2f1c8c0-57d1-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E103" t="str">
+        <v>soporte@eilsa.mx</v>
+      </c>
+      <c r="F103">
+        <v>1695329202</v>
+      </c>
+      <c r="G103" t="str">
+        <v>f83ab3a0-58bf-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H103" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I103" s="1">
+        <v>45190.615375636575</v>
+      </c>
+      <c r="J103" s="1">
+        <v>45190.615375636575</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>883e2766-94aa-40d4-b1b8-eaaa3bb05371</v>
+      </c>
+      <c r="B104" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C104" t="str">
+        <v/>
+      </c>
+      <c r="D104" t="str">
+        <v>524a2c40-58bd-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E104" t="str">
+        <v>compras4@farmaciassanasana.com.mx</v>
+      </c>
+      <c r="F104">
+        <v>1695328064</v>
+      </c>
+      <c r="G104" t="str">
+        <v>524b0492-58bd-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H104" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I104" s="1">
+        <v>45190.60252512732</v>
+      </c>
+      <c r="J104" s="1">
+        <v>45190.60252512732</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>d525ad61-6693-4c2e-83e2-9577843e676a</v>
+      </c>
+      <c r="B105" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C105" t="str">
+        <v/>
+      </c>
+      <c r="D105" t="str">
+        <v>524ceb60-58bd-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E105" t="str">
+        <v>gerente.comercial@farmaciassanasana.com.mx</v>
+      </c>
+      <c r="F105">
+        <v>1695328064</v>
+      </c>
+      <c r="G105" t="str">
+        <v>524dfa65-58bd-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H105" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I105" s="1">
+        <v>45190.60252540509</v>
+      </c>
+      <c r="J105" s="1">
+        <v>45190.60252540509</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>b511f36a-8788-4410-8d14-7bc056ad8c05</v>
+      </c>
+      <c r="B106" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C106" t="str">
+        <v/>
+      </c>
+      <c r="D106" t="str">
+        <v>b17e3a80-58c7-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E106" t="str">
+        <v>centrodcontrol@segutridadesa.com.mx</v>
+      </c>
+      <c r="F106">
+        <v>1695332519</v>
+      </c>
+      <c r="G106" t="str">
+        <v>b17ee446-58c7-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H106" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I106" s="1">
+        <v>45190.653904039355</v>
+      </c>
+      <c r="J106" s="1">
+        <v>45190.653904039355</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>10c32012-c6c6-4f5f-ae31-99a634bf73a8</v>
+      </c>
+      <c r="B107" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C107" t="str">
+        <v/>
+      </c>
+      <c r="D107" t="str">
+        <v>e4b9f740-58bd-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E107" t="str">
+        <v>jclopez@circuloavl.com</v>
+      </c>
+      <c r="F107">
+        <v>1695328310</v>
+      </c>
+      <c r="G107" t="str">
+        <v>e4baa65c-58bd-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H107" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I107" s="1">
+        <v>45190.60530256944</v>
+      </c>
+      <c r="J107" s="1">
+        <v>45190.60530256944</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>1eca5748-4bae-4a06-986c-315ea0f8dc79</v>
+      </c>
+      <c r="B108" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C108" t="str">
+        <v/>
+      </c>
+      <c r="D108" t="str">
+        <v>31126870-57d3-11ee-0040-f17e2c986ab3</v>
+      </c>
+      <c r="E108" t="str">
+        <v>telcelalarmas@gmail.com</v>
+      </c>
+      <c r="F108">
+        <v>1695329866</v>
+      </c>
+      <c r="G108" t="str">
+        <v>847d58bf-58c1-11ee-81bf-0a58a9feac02</v>
+      </c>
+      <c r="H108" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I108" s="1">
+        <v>45190.623358020835</v>
+      </c>
+      <c r="J108" s="1">
+        <v>45190.623358020835</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>5df149d6-46a9-48d6-9f06-49fcdfab6d5f</v>
+      </c>
+      <c r="B109" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C109" t="str">
+        <v/>
+      </c>
+      <c r="D109" t="str">
+        <v>55569e40-57d3-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E109" t="str">
+        <v>sevilimex.monitoreo@gmail.com</v>
+      </c>
+      <c r="F109">
+        <v>1695329927</v>
+      </c>
+      <c r="G109" t="str">
+        <v>a8bcb164-58c1-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H109" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I109" s="1">
+        <v>45190.6240531713</v>
+      </c>
+      <c r="J109" s="1">
+        <v>45190.6240531713</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>d12541cd-a2a7-4d8c-942c-35950b09ce43</v>
+      </c>
+      <c r="B110" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C110" t="str">
+        <v/>
+      </c>
+      <c r="D110" t="str">
+        <v>5557afb0-57d3-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E110" t="str">
+        <v>karenmaudhik3@gmail.com</v>
+      </c>
+      <c r="F110">
+        <v>1695329927</v>
+      </c>
+      <c r="G110" t="str">
+        <v>a8bd60f3-58c1-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H110" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I110" s="1">
+        <v>45190.62405337963</v>
+      </c>
+      <c r="J110" s="1">
+        <v>45190.62405337963</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>84758a6b-de9b-4729-bbae-7a82dabb7821</v>
+      </c>
+      <c r="B111" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C111" t="str">
+        <v/>
+      </c>
+      <c r="D111" t="str">
+        <v>555fed10-57d3-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E111" t="str">
+        <v>alejandra.tanaka@monfel.com</v>
+      </c>
+      <c r="F111">
+        <v>1695329927</v>
+      </c>
+      <c r="G111" t="str">
+        <v>a8c76fd1-58c1-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H111" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I111" s="1">
+        <v>45190.62405342593</v>
+      </c>
+      <c r="J111" s="1">
+        <v>45190.62405342593</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>45862416-9126-4429-a545-732c836b8703</v>
+      </c>
+      <c r="B112" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C112" t="str">
+        <v/>
+      </c>
+      <c r="D112" t="str">
+        <v>5560b060-57d3-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E112" t="str">
+        <v>veronica.gallegos@monfel.com</v>
+      </c>
+      <c r="F112">
+        <v>1695329927</v>
+      </c>
+      <c r="G112" t="str">
+        <v>a8c4e9c4-58c1-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H112" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I112" s="1">
+        <v>45190.624053472224</v>
+      </c>
+      <c r="J112" s="1">
+        <v>45190.624053472224</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>def191a6-ea74-40da-8ae9-ee50da0a86ea</v>
+      </c>
+      <c r="B113" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C113" t="str">
+        <v/>
+      </c>
+      <c r="D113" t="str">
+        <v>55674010-57d3-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E113" t="str">
+        <v>granos@grupoansa.mx</v>
+      </c>
+      <c r="F113">
+        <v>1695329927</v>
+      </c>
+      <c r="G113" t="str">
+        <v>a8d2cf97-58c1-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H113" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I113" s="1">
+        <v>45190.624053506945</v>
+      </c>
+      <c r="J113" s="1">
+        <v>45190.624053506945</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>d93dc1d3-fb3c-4d3a-aec9-8d66a29dff08</v>
+      </c>
+      <c r="B114" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C114" t="str">
+        <v/>
+      </c>
+      <c r="D114" t="str">
+        <v>675bced0-57d3-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E114" t="str">
+        <v>auxoperacionesmartins@gmail.com</v>
+      </c>
+      <c r="F114">
+        <v>1695329958</v>
+      </c>
+      <c r="G114" t="str">
+        <v>bac55eab-58c1-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H114" t="str">
+        <v>hourly_rate_exceeded</v>
+      </c>
+      <c r="I114" s="1">
+        <v>45190.62440289352</v>
+      </c>
+      <c r="J114" s="1">
+        <v>45190.62440289352</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>61288119-dc55-4923-b8e8-d80224398e2b</v>
+      </c>
+      <c r="B115" t="str">
+        <v>reject</v>
+      </c>
+      <c r="C115" t="str">
+        <v/>
+      </c>
+      <c r="D115" t="str">
+        <v>5c3cb550-58c8-11ee-0000-f1c69420d20b</v>
+      </c>
+      <c r="E115" t="str">
+        <v>administracion@lalomuebleria.com</v>
+      </c>
+      <c r="F115">
+        <v>1695332805</v>
+      </c>
+      <c r="G115" t="str">
+        <v>5c3d5ecb-58c8-11ee-8862-0a58a9feac02</v>
+      </c>
+      <c r="H115" t="str">
+        <v>hard bounce</v>
+      </c>
+      <c r="I115" s="1">
+        <v>45190.65738853009</v>
+      </c>
+      <c r="J115" s="1">
+        <v>45190.65738853009</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J28"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J115"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>